<commit_message>
feat: update subsidy application plans with revised Excel files
</commit_message>
<xml_diff>
--- a/docs/plans/001-subsidy-application/旅遊補助.xlsx
+++ b/docs/plans/001-subsidy-application/旅遊補助.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wengshengkai/projects/side-project/NGEip/docs/plans/001-subsidy-application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA54DEE3-1AE6-474A-934A-45198B3FD99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F6FAEF-2505-FC4C-AC65-6823A0DF6C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="1340" windowWidth="27840" windowHeight="16820" xr2:uid="{9FD17495-6405-EB48-B7F1-D9C0EFBC3FBD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>莊栢瑞</t>
   </si>
@@ -47,15 +47,9 @@
     <t>凃皓景</t>
   </si>
   <si>
-    <t>成天惠</t>
-  </si>
-  <si>
     <t>吳奇燊</t>
   </si>
   <si>
-    <t>陳毅豪</t>
-  </si>
-  <si>
     <t>黃祿芸</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>徐嘉言</t>
   </si>
   <si>
-    <t>吳思昀</t>
-  </si>
-  <si>
     <t>陳力卉</t>
   </si>
   <si>
@@ -84,87 +75,6 @@
   </si>
   <si>
     <t>何叡昇</t>
-  </si>
-  <si>
-    <t>王庭恩</t>
-  </si>
-  <si>
-    <t>鄭仲智</t>
-  </si>
-  <si>
-    <t>蕭逸芬</t>
-  </si>
-  <si>
-    <t>陳玟宇</t>
-  </si>
-  <si>
-    <t>張叔安</t>
-  </si>
-  <si>
-    <t>簡珮珊</t>
-  </si>
-  <si>
-    <t>張巧儒</t>
-  </si>
-  <si>
-    <t>周棋</t>
-  </si>
-  <si>
-    <t>張修豪</t>
-  </si>
-  <si>
-    <t>鄭淯心</t>
-  </si>
-  <si>
-    <t>陳凱翔</t>
-  </si>
-  <si>
-    <t>林沛珊</t>
-  </si>
-  <si>
-    <t>李威辰</t>
-  </si>
-  <si>
-    <t>鄧仕良</t>
-  </si>
-  <si>
-    <t>許惟棠</t>
-  </si>
-  <si>
-    <t>李智鈞</t>
-  </si>
-  <si>
-    <t>林佩蓁</t>
-  </si>
-  <si>
-    <t>胡裕晟</t>
-  </si>
-  <si>
-    <t>孫雅亭</t>
-  </si>
-  <si>
-    <t>陳羽絹</t>
-  </si>
-  <si>
-    <t>蔡彣山</t>
-  </si>
-  <si>
-    <t>張珉豪</t>
-  </si>
-  <si>
-    <t>彭志全</t>
-  </si>
-  <si>
-    <t>方宜姍</t>
-  </si>
-  <si>
-    <t>田凱卉</t>
-  </si>
-  <si>
-    <t>陳瑤芝</t>
-  </si>
-  <si>
-    <t>侯蘊芸</t>
   </si>
   <si>
     <t>姓名</t>
@@ -199,23 +109,31 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>個人旅遊</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t>2025</t>
+      <t>2023</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
+        <family val="3"/>
+        <charset val="136"/>
       </rPr>
-      <t>員旅</t>
+      <t>員旅台南</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>2023員旅台南</t>
+  </si>
+  <si>
     <r>
-      <t>2025</t>
+      <t>2023</t>
     </r>
     <r>
       <rPr>
@@ -226,54 +144,15 @@
         <charset val="136"/>
         <scheme val="minor"/>
       </rPr>
-      <t>員旅</t>
+      <t>員旅台南</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>2024</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>員旅</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>2024</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>員旅</t>
-    </r>
-  </si>
-  <si>
-    <t>個人旅遊</t>
-  </si>
-  <si>
-    <t>個人旅遊</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -294,12 +173,6 @@
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -332,22 +205,16 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Microsoft JhengHei"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -389,24 +256,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -625,889 +487,330 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1023"/>
+  <dimension ref="A1:D973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>50</v>
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="11">
-        <v>45650</v>
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8">
+        <v>45094</v>
       </c>
       <c r="C2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>56</v>
+        <v>13159</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="11">
-        <v>45929</v>
+      <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="9">
+        <v>45094</v>
       </c>
       <c r="C3" s="3">
-        <v>38900</v>
+        <v>13159</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="11">
-        <v>45383</v>
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9">
+        <v>45094</v>
       </c>
       <c r="C4" s="3">
-        <v>32300</v>
+        <v>13159</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C5" s="3">
-        <v>38900</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9">
+        <v>45094</v>
+      </c>
+      <c r="C5" s="1">
+        <v>13159</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="12">
-        <v>45505</v>
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="9">
+        <v>45094</v>
       </c>
       <c r="C6" s="3">
-        <v>10000</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="11">
-        <v>45849</v>
-      </c>
-      <c r="C7" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>55</v>
+        <v>13159</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <v>45094</v>
+      </c>
+      <c r="C7" s="3">
+        <v>13159</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C8" s="1">
-        <v>32300</v>
+        <v>2</v>
+      </c>
+      <c r="B8" s="9">
+        <v>45094</v>
+      </c>
+      <c r="C8" s="3">
+        <v>13159</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C9" s="1">
-        <v>32300</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8">
+        <v>45094</v>
+      </c>
+      <c r="C9" s="3">
+        <v>13159</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="12">
-        <v>45929</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="8">
+        <v>45094</v>
       </c>
       <c r="C10" s="3">
-        <v>38900</v>
+        <v>13159</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C11" s="3">
-        <v>32300</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>45094</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13159</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="12">
-        <v>45974</v>
-      </c>
-      <c r="C12" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45094</v>
+      </c>
+      <c r="C12" s="3">
+        <v>13159</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="12">
-        <v>45383</v>
+        <v>7</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45094</v>
       </c>
       <c r="C13" s="3">
-        <v>32300</v>
+        <v>13159</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="12">
-        <v>45929</v>
+        <v>8</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45094</v>
       </c>
       <c r="C14" s="3">
-        <v>38900</v>
+        <v>13159</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="11">
-        <v>45648</v>
+        <v>9</v>
+      </c>
+      <c r="B15" s="10">
+        <v>45094</v>
       </c>
       <c r="C15" s="1">
-        <v>9450</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>55</v>
+        <v>13159</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="11">
-        <v>45383</v>
+        <v>10</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45094</v>
       </c>
       <c r="C16" s="3">
-        <v>32300</v>
+        <v>13159</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C17" s="3">
-        <v>38900</v>
+        <v>11</v>
+      </c>
+      <c r="B17" s="9">
+        <v>45094</v>
+      </c>
+      <c r="C17" s="2">
+        <v>13159</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="11">
-        <v>45544</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3000</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="11">
-        <v>45383</v>
-      </c>
-      <c r="C19" s="3">
-        <v>32300</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C20" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="11">
-        <v>45388</v>
-      </c>
-      <c r="C21" s="1">
-        <v>10000</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
+        <v>12</v>
+      </c>
+      <c r="B18" s="9">
+        <v>45094</v>
+      </c>
+      <c r="C18" s="3">
+        <v>13159</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
     <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="11">
-        <v>45383</v>
-      </c>
-      <c r="C22" s="1">
-        <v>32300</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C23" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C24" s="3">
-        <v>32300</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C25" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C26" s="3">
-        <v>32300</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C27" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="13">
-        <v>45383</v>
-      </c>
-      <c r="C29" s="1">
-        <v>32300</v>
-      </c>
-      <c r="D29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C30" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C31" s="3">
-        <v>32300</v>
-      </c>
-      <c r="D31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="12">
-        <v>45887</v>
-      </c>
-      <c r="C32" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C33" s="2">
-        <v>32300</v>
-      </c>
-      <c r="D33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C34" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C35" s="3">
-        <v>32300</v>
-      </c>
-      <c r="D35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" s="12">
-        <v>45902</v>
-      </c>
-      <c r="C36" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C37" s="2">
-        <v>32300</v>
-      </c>
-      <c r="D37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="12">
-        <v>45825</v>
-      </c>
-      <c r="C38" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C39" s="1">
-        <v>32300</v>
-      </c>
-      <c r="D39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="11">
-        <v>45535</v>
-      </c>
-      <c r="C40" s="1">
-        <v>10000</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="11">
-        <v>45383</v>
-      </c>
-      <c r="C41" s="1">
-        <v>32300</v>
-      </c>
-      <c r="D41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C42" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D42" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="13">
-        <v>45383</v>
-      </c>
-      <c r="C44" s="1">
-        <v>32300</v>
-      </c>
-      <c r="D44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C45" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D45" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C46" s="3">
-        <v>32300</v>
-      </c>
-      <c r="D46" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A47" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C47" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D47" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A48" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B48" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C48" s="1">
-        <v>32300</v>
-      </c>
-      <c r="D48" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="12">
-        <v>45383</v>
-      </c>
-      <c r="C49" s="1">
-        <v>32300</v>
-      </c>
-      <c r="D49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="12">
-        <v>45929</v>
-      </c>
-      <c r="C50" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="13">
-        <v>45966</v>
-      </c>
-      <c r="C51" s="2">
-        <v>6819</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="12">
-        <v>45902</v>
-      </c>
-      <c r="C52" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B53" s="12">
-        <v>45924</v>
-      </c>
-      <c r="C53" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B54" s="13">
-        <v>45929</v>
-      </c>
-      <c r="C54" s="3">
-        <v>38900</v>
-      </c>
-      <c r="D54" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="13">
-        <v>45929</v>
-      </c>
-      <c r="C56" s="3">
-        <v>33916</v>
-      </c>
-      <c r="D56" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A58" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A59" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="13">
-        <v>45929</v>
-      </c>
-      <c r="C59" s="3">
-        <v>24191</v>
-      </c>
-      <c r="D59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A60" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A61" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B61" s="13">
-        <v>45929</v>
-      </c>
-      <c r="C61" s="3">
-        <v>20950</v>
-      </c>
-      <c r="D61" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A62" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A63" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A64" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A65" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A66" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A67" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="70" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="72" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A72" s="7"/>
-    </row>
-    <row r="73" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="74" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="75" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="76" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="77" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="78" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="79" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="80" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="55" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="56" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="57" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="58" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="59" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="60" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="61" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="62" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="63" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="64" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="13" x14ac:dyDescent="0.15"/>
     <row r="81" ht="13" x14ac:dyDescent="0.15"/>
     <row r="82" ht="13" x14ac:dyDescent="0.15"/>
     <row r="83" ht="13" x14ac:dyDescent="0.15"/>
@@ -2401,56 +1704,6 @@
     <row r="971" ht="13" x14ac:dyDescent="0.15"/>
     <row r="972" ht="13" x14ac:dyDescent="0.15"/>
     <row r="973" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1001" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1002" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1003" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1004" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1005" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1006" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1007" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1008" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1009" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1010" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1011" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1012" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1013" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1014" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1015" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1016" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1017" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1018" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1019" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1020" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1021" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1022" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1023" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>